<commit_message>
Fix issue with external scenario
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-synfuels-from-FT-from-natural-gas.xlsx
+++ b/premise/data/additional_inventories/lci-synfuels-from-FT-from-natural-gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924D9E2F-9BAA-E346-9BA0-8C1E6C663200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8933A371-2701-5C4C-A76D-C7F862BFEA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>market for natural gas, low pressure</t>
   </si>
   <si>
-    <t>RoE</t>
-  </si>
-  <si>
     <t>natural gas, low pressure</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>liquefied petroleum gas production, synthetic, Fischer Tropsch process, from natural gas, energy allocation, with carbon capture and storage</t>
+  </si>
+  <si>
+    <t>RoW</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1412,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>2.1</v>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1738,7 +1738,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32">
         <v>2.35</v>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1871,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1966,7 +1966,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50">
         <v>2.3199999999999998</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54">
         <v>0.19</v>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2172,7 +2172,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2187,12 +2187,12 @@
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68">
         <v>2.2599999999999998</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72">
         <v>0.05</v>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2325,7 +2325,7 @@
         <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2357,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2365,7 +2365,7 @@
         <v>25</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2421,12 +2421,12 @@
         <v>liquefied petroleum gas production, synthetic, Fischer Tropsch process, from natural gas, energy allocation</v>
       </c>
       <c r="H85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86">
         <v>2.2799999999999998</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B90">
         <v>0.13</v>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2591,7 +2591,7 @@
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -2664,7 +2664,7 @@
         <v>2.0272108843537415</v>
       </c>
       <c r="C104" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D104" t="s">
         <v>20</v>
@@ -2673,15 +2673,15 @@
         <v>16</v>
       </c>
       <c r="G104" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H104" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B105" s="16">
         <f>4.1-1.375</f>
@@ -2700,7 +2700,7 @@
         <v>19</v>
       </c>
       <c r="H105" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2708,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -2724,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -2819,7 +2819,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B118">
         <v>2.1</v>
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -3050,7 +3050,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B136">
         <v>2.35</v>
@@ -3167,7 +3167,7 @@
         <v>0</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -3183,7 +3183,7 @@
         <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
@@ -3278,7 +3278,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B154">
         <v>2.3199999999999998</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B158">
         <v>0.19</v>
@@ -3395,7 +3395,7 @@
         <v>0</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -3411,7 +3411,7 @@
         <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -3500,12 +3500,12 @@
         <v>15</v>
       </c>
       <c r="G171" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B172">
         <v>2.2599999999999998</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B176">
         <v>0.05</v>
@@ -3622,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -3638,7 +3638,7 @@
         <v>2</v>
       </c>
       <c r="B181" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -3670,7 +3670,7 @@
         <v>9</v>
       </c>
       <c r="B185" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -3678,7 +3678,7 @@
         <v>25</v>
       </c>
       <c r="B186" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3734,12 +3734,12 @@
         <v>liquefied petroleum gas production, synthetic, Fischer Tropsch process, from natural gas, energy allocation, with carbon capture and storage</v>
       </c>
       <c r="H189" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B190">
         <v>2.2799999999999998</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B194">
         <v>0.13</v>
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -3904,7 +3904,7 @@
         <v>9</v>
       </c>
       <c r="B203" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -3977,7 +3977,7 @@
         <v>2.0272108843537415</v>
       </c>
       <c r="C208" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D208" t="s">
         <v>20</v>
@@ -3986,15 +3986,15 @@
         <v>16</v>
       </c>
       <c r="G208" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H208" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B209" s="16">
         <f>(4.1-1.375)*0.01</f>
@@ -4013,7 +4013,7 @@
         <v>19</v>
       </c>
       <c r="H209" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4037,12 +4037,12 @@
         <v>23</v>
       </c>
       <c r="H210" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B211" s="16">
         <f>(4.1-1.375)*0.99</f>
@@ -4058,7 +4058,7 @@
         <v>16</v>
       </c>
       <c r="G211" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="217" spans="1:8" ht="16" x14ac:dyDescent="0.2">

</xml_diff>